<commit_message>
Tests & bug fix
</commit_message>
<xml_diff>
--- a/apps/backend/tests/test_files/test_one_step_2022_05_Май_2-12176-pentadal_forecast_bulletin.xlsx
+++ b/apps/backend/tests/test_files/test_one_step_2022_05_Май_2-12176-pentadal_forecast_bulletin.xlsx
@@ -2701,11 +2701,7 @@
         </is>
       </c>
       <c r="B8" s="21" t="inlineStr"/>
-      <c r="C8" s="22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C8" s="22" t="inlineStr"/>
       <c r="D8" s="7" t="n"/>
       <c r="E8" s="6" t="n"/>
       <c r="F8" s="6" t="n"/>

</xml_diff>

<commit_message>
Fix rounding of hydrol. data part 1
Rounding of discharge is now to 3 numbers as typically used. Still need to check the output after pseudo-operational run
</commit_message>
<xml_diff>
--- a/apps/backend/tests/test_files/test_one_step_2022_05_Май_2-12176-pentadal_forecast_bulletin.xlsx
+++ b/apps/backend/tests/test_files/test_one_step_2022_05_Май_2-12176-pentadal_forecast_bulletin.xlsx
@@ -2594,12 +2594,12 @@
       </c>
       <c r="B4" s="21" t="inlineStr">
         <is>
-          <t>4,3200</t>
+          <t>4,32</t>
         </is>
       </c>
       <c r="C4" s="22" t="inlineStr">
         <is>
-          <t>17,1100</t>
+          <t>17,1</t>
         </is>
       </c>
       <c r="D4" s="7" t="n"/>
@@ -2621,12 +2621,12 @@
       </c>
       <c r="B5" s="21" t="inlineStr">
         <is>
-          <t>4,6280</t>
+          <t>4,63</t>
         </is>
       </c>
       <c r="C5" s="22" t="inlineStr">
         <is>
-          <t>16,5700</t>
+          <t>16,6</t>
         </is>
       </c>
       <c r="D5" s="7" t="n"/>
@@ -2648,12 +2648,12 @@
       </c>
       <c r="B6" s="21" t="inlineStr">
         <is>
-          <t>5,3540</t>
+          <t>5,35</t>
         </is>
       </c>
       <c r="C6" s="22" t="inlineStr">
         <is>
-          <t>19,0800</t>
+          <t>19,1</t>
         </is>
       </c>
       <c r="D6" s="7" t="n"/>
@@ -2675,12 +2675,12 @@
       </c>
       <c r="B7" s="21" t="inlineStr">
         <is>
-          <t>8,0100</t>
+          <t>8,01</t>
         </is>
       </c>
       <c r="C7" s="22" t="inlineStr">
         <is>
-          <t>15,2100</t>
+          <t>15,2</t>
         </is>
       </c>
       <c r="D7" s="7" t="n"/>

</xml_diff>